<commit_message>
update software schedule (again)
</commit_message>
<xml_diff>
--- a/Phase2-3/Software Development Schedule.xlsx
+++ b/Phase2-3/Software Development Schedule.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="47">
   <si>
     <t>Materials, Traps, Weapons, Minor Objectives will probably have definitive start and end tasks. Player and AI classes will probably be continuously updated to integrate the other objects.</t>
   </si>
@@ -70,7 +70,7 @@
     <t>Game demonstration.</t>
   </si>
   <si>
-    <t>Add skeletal mesh to player pawn.</t>
+    <t>Add skeletal mesh to player pawn; update project defaults to select game mode and pawn.</t>
   </si>
   <si>
     <t>Screenshot of skeletal mesh attached to player pawn.</t>
@@ -586,6 +586,9 @@
       <c r="B14" s="5" t="s">
         <v>17</v>
       </c>
+      <c r="C14" s="6" t="s">
+        <v>11</v>
+      </c>
       <c r="D14" s="6" t="s">
         <v>18</v>
       </c>
@@ -599,6 +602,9 @@
       <c r="B16" s="11" t="s">
         <v>19</v>
       </c>
+      <c r="C16" s="6" t="s">
+        <v>9</v>
+      </c>
       <c r="D16" s="6" t="s">
         <v>20</v>
       </c>
@@ -611,6 +617,9 @@
       <c r="A18" s="4"/>
       <c r="B18" s="11" t="s">
         <v>21</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>13</v>
       </c>
       <c r="D18" s="6" t="s">
         <v>18</v>

</xml_diff>

<commit_message>
update software schedule with this week's tasks
</commit_message>
<xml_diff>
--- a/Phase2-3/Software Development Schedule.xlsx
+++ b/Phase2-3/Software Development Schedule.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="55">
   <si>
     <t>Materials, Traps, Weapons, Minor Objectives will probably have definitive start and end tasks. Player and AI classes will probably be continuously updated to integrate the other objects.</t>
   </si>
@@ -67,49 +67,73 @@
     <t>Start building the level according to the bird's eye view.</t>
   </si>
   <si>
+    <t>Game demonstration of sculpted landscape.</t>
+  </si>
+  <si>
+    <t>Present bird's-eye view diagram of level.</t>
+  </si>
+  <si>
+    <t>Add skeletal mesh to player pawn; update project defaults to select game mode and pawn.</t>
+  </si>
+  <si>
+    <t>Screenshot of skeletal mesh attached to player pawn.</t>
+  </si>
+  <si>
+    <t>Make player pawn move around and jump.</t>
+  </si>
+  <si>
     <t>Game demonstration.</t>
   </si>
   <si>
-    <t>Add skeletal mesh to player pawn; update project defaults to select game mode and pawn.</t>
-  </si>
-  <si>
-    <t>Screenshot of skeletal mesh attached to player pawn.</t>
-  </si>
-  <si>
-    <t>Make player pawn move around and jump.</t>
-  </si>
-  <si>
-    <t>Create a material actor. Allow player to interact w/ material.</t>
-  </si>
-  <si>
     <t>Create AI pawn. Have it follow player.</t>
   </si>
   <si>
     <t>2/7 - 2/14</t>
   </si>
   <si>
-    <t>Create more variety of materials. Create material set for game.</t>
-  </si>
-  <si>
-    <t>Screenshot or code</t>
-  </si>
-  <si>
-    <t>Add functionality to check if material is brought to a specific location.</t>
+    <t>Create a Material, have player be able to walk over and interact with it</t>
+  </si>
+  <si>
+    <t>Output log when walking over</t>
+  </si>
+  <si>
+    <t>Implement basic AI Behavior Tree</t>
+  </si>
+  <si>
+    <t>Screenshot</t>
+  </si>
+  <si>
+    <t>Animate Player and AI models</t>
   </si>
   <si>
     <t>Game demonstration</t>
   </si>
   <si>
-    <t>Have AI scout prioritize locations with materials.</t>
-  </si>
-  <si>
     <t>Add details, lighting, etc. to map.</t>
   </si>
   <si>
+    <t xml:space="preserve">Present screenshot of UE bird's-eye view of the map </t>
+  </si>
+  <si>
+    <t>(to showcase area divisions). Also game demonstration.</t>
+  </si>
+  <si>
     <t>2/14 - 2/21</t>
   </si>
   <si>
-    <t>Finish Material, Start Minor Objective</t>
+    <t>Expand AI Behavior Tree to scout for material locations</t>
+  </si>
+  <si>
+    <t>Implement a check for materials when player is in crafting location, allow materials to respawn if "dropped"</t>
+  </si>
+  <si>
+    <t>Start minor objectives</t>
+  </si>
+  <si>
+    <t>Anthony</t>
+  </si>
+  <si>
+    <t>Add details, lighting, etc. to map</t>
   </si>
   <si>
     <t>2/21 - 2/28</t>
@@ -470,9 +494,9 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="16.0"/>
-    <col customWidth="1" min="2" max="2" width="66.57"/>
-    <col customWidth="1" min="3" max="3" width="44.0"/>
+    <col customWidth="1" min="1" max="1" width="10.57"/>
+    <col customWidth="1" min="2" max="2" width="44.86"/>
+    <col customWidth="1" min="3" max="3" width="12.43"/>
     <col customWidth="1" min="4" max="4" width="52.29"/>
   </cols>
   <sheetData>
@@ -596,17 +620,20 @@
     <row r="15">
       <c r="A15" s="4"/>
       <c r="B15" s="5"/>
+      <c r="D15" s="6" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="4"/>
       <c r="B16" s="11" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C16" s="6" t="s">
         <v>9</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="17">
@@ -616,13 +643,13 @@
     <row r="18">
       <c r="A18" s="4"/>
       <c r="B18" s="11" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C18" s="6" t="s">
         <v>13</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
     </row>
     <row r="19">
@@ -632,104 +659,108 @@
     <row r="20">
       <c r="A20" s="4"/>
       <c r="B20" s="11" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C20" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="4"/>
-      <c r="B21" s="11"/>
+      <c r="A21" s="7"/>
+      <c r="B21" s="12"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="13"/>
     </row>
     <row r="22">
-      <c r="A22" s="4"/>
-      <c r="B22" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="C22" s="6" t="s">
+      <c r="A22" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B22" s="10"/>
+    </row>
+    <row r="23">
+      <c r="A23" s="4"/>
+      <c r="B23" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C23" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D22" s="6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="7"/>
-      <c r="B23" s="12"/>
-      <c r="C23" s="13"/>
-      <c r="D23" s="13"/>
+      <c r="D23" s="6" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="24">
-      <c r="A24" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B24" s="10"/>
+      <c r="A24" s="4"/>
+      <c r="B24" s="5"/>
+      <c r="D24" s="6"/>
     </row>
     <row r="25">
       <c r="A25" s="4"/>
       <c r="B25" s="5" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="4"/>
       <c r="B26" s="5"/>
-      <c r="D26" s="6"/>
     </row>
     <row r="27">
       <c r="A27" s="4"/>
       <c r="B27" s="5" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="4"/>
       <c r="B28" s="5"/>
+      <c r="D28" s="6"/>
     </row>
     <row r="29">
       <c r="A29" s="4"/>
       <c r="B29" s="5" t="s">
-        <v>29</v>
+        <v>32</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>11</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="4"/>
-      <c r="B30" s="5"/>
-      <c r="D30" s="6"/>
+      <c r="D30" s="6" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="31">
-      <c r="A31" s="4"/>
-      <c r="B31" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="D31" s="6" t="s">
-        <v>28</v>
-      </c>
+      <c r="A31" s="7"/>
+      <c r="B31" s="12"/>
+      <c r="C31" s="13"/>
+      <c r="D31" s="13"/>
     </row>
     <row r="32">
-      <c r="A32" s="7"/>
-      <c r="B32" s="12"/>
-      <c r="C32" s="13"/>
-      <c r="D32" s="13"/>
+      <c r="A32" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B32" s="10"/>
     </row>
     <row r="33">
-      <c r="A33" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="B33" s="10"/>
+      <c r="A33" s="4"/>
+      <c r="B33" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="4"/>
@@ -738,95 +769,134 @@
     <row r="35">
       <c r="A35" s="4"/>
       <c r="B35" s="5" t="s">
-        <v>32</v>
+        <v>37</v>
+      </c>
+      <c r="C35" s="6" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B36" s="10"/>
+      <c r="A36" s="4"/>
+      <c r="B36" s="5"/>
     </row>
     <row r="37">
       <c r="A37" s="4"/>
-      <c r="B37" s="5"/>
+      <c r="B37" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="38">
-      <c r="A38" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B38" s="10"/>
+      <c r="A38" s="4"/>
+      <c r="B38" s="5"/>
     </row>
     <row r="39">
-      <c r="A39" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B39" s="10"/>
+      <c r="A39" s="4"/>
+      <c r="B39" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C39" s="6" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" s="4"/>
-      <c r="B40" s="5" t="s">
-        <v>36</v>
-      </c>
+      <c r="B40" s="10"/>
     </row>
     <row r="41">
-      <c r="A41" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B41" s="10"/>
+      <c r="A41" s="7"/>
+      <c r="B41" s="12"/>
+      <c r="C41" s="13"/>
+      <c r="D41" s="13"/>
     </row>
     <row r="42">
       <c r="A42" s="4" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B42" s="10"/>
     </row>
     <row r="43">
-      <c r="A43" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="B43" s="10"/>
+      <c r="A43" s="4"/>
+      <c r="B43" s="5"/>
     </row>
     <row r="44">
-      <c r="A44" s="4"/>
-      <c r="B44" s="5" t="s">
-        <v>40</v>
-      </c>
+      <c r="A44" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B44" s="10"/>
     </row>
     <row r="45">
       <c r="A45" s="4" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B45" s="10"/>
     </row>
     <row r="46">
-      <c r="A46" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="B46" s="10"/>
+      <c r="A46" s="4"/>
+      <c r="B46" s="5" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" s="4" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B47" s="10"/>
     </row>
     <row r="48">
-      <c r="A48" s="4"/>
-      <c r="B48" s="5" t="s">
-        <v>44</v>
-      </c>
+      <c r="A48" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B48" s="10"/>
     </row>
     <row r="49">
       <c r="A49" s="4" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B49" s="10"/>
     </row>
     <row r="50">
       <c r="A50" s="4"/>
       <c r="B50" s="5" t="s">
-        <v>46</v>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B51" s="10"/>
+    </row>
+    <row r="52">
+      <c r="A52" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B52" s="10"/>
+    </row>
+    <row r="53">
+      <c r="A53" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B53" s="10"/>
+    </row>
+    <row r="54">
+      <c r="A54" s="4"/>
+      <c r="B54" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B55" s="10"/>
+    </row>
+    <row r="56">
+      <c r="A56" s="4"/>
+      <c r="B56" s="5" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>